<commit_message>
add John to roster
</commit_message>
<xml_diff>
--- a/tf-dev-vm-access.xlsx
+++ b/tf-dev-vm-access.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jruels/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E9389E-9971-6B4B-B3DA-4D7C54E1B5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D8EB4A-A433-7142-9AD9-2323DE4D3885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="4560" windowWidth="35360" windowHeight="18160" xr2:uid="{17AF21C6-E61B-994C-83EC-C5D121A671AF}"/>
+    <workbookView xWindow="1560" yWindow="2560" windowWidth="35360" windowHeight="18160" xr2:uid="{17AF21C6-E61B-994C-83EC-C5D121A671AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="117">
   <si>
     <t>Virtual Machine Password</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Muppala</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>White</t>
   </si>
   <si>
     <t>Rakesh</t>
@@ -826,7 +832,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,256 +846,256 @@
   <sheetData>
     <row r="1" spans="1:17" ht="27" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="27" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="7" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26" x14ac:dyDescent="0.3">
@@ -1101,12 +1107,18 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="D22" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1138,24 +1150,24 @@
   <sheetData>
     <row r="1" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M1" s="5"/>
     </row>
@@ -1164,37 +1176,37 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1203,19 +1215,19 @@
     </row>
     <row r="4" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -1224,19 +1236,19 @@
     </row>
     <row r="5" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -1245,19 +1257,19 @@
     </row>
     <row r="6" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -1266,19 +1278,19 @@
     </row>
     <row r="7" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -1287,19 +1299,19 @@
     </row>
     <row r="8" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -1308,19 +1320,19 @@
     </row>
     <row r="9" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -1329,19 +1341,19 @@
     </row>
     <row r="10" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -1350,19 +1362,19 @@
     </row>
     <row r="11" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -1371,19 +1383,19 @@
     </row>
     <row r="12" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -1392,19 +1404,19 @@
     </row>
     <row r="13" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -1413,19 +1425,19 @@
     </row>
     <row r="14" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -1434,19 +1446,19 @@
     </row>
     <row r="15" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -1455,19 +1467,19 @@
     </row>
     <row r="16" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -1476,19 +1488,19 @@
     </row>
     <row r="17" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -1497,19 +1509,19 @@
     </row>
     <row r="18" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -1518,19 +1530,19 @@
     </row>
     <row r="19" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -1539,19 +1551,19 @@
     </row>
     <row r="20" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -1560,19 +1572,19 @@
     </row>
     <row r="21" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -1581,19 +1593,19 @@
     </row>
     <row r="22" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>

</xml_diff>

<commit_message>
typo - John is machine 20
</commit_message>
<xml_diff>
--- a/tf-dev-vm-access.xlsx
+++ b/tf-dev-vm-access.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jruels/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BAEF94-5638-FC4C-A31D-CFA4CD09504B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9434E3A3-E34E-3F4E-9F0E-CFA0A7BBE539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="5260" windowWidth="35360" windowHeight="18160" xr2:uid="{17AF21C6-E61B-994C-83EC-C5D121A671AF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="114">
   <si>
     <t>Virtual Machine Password</t>
   </si>
@@ -379,9 +379,6 @@
   </si>
   <si>
     <t>WNS2022-20</t>
-  </si>
-  <si>
-    <t>WNS2022-21</t>
   </si>
 </sst>
 </file>
@@ -846,7 +843,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1125,9 +1122,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="D22" s="8" t="s">
-        <v>114</v>
-      </c>
+      <c r="D22" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>